<commit_message>
added solutions and bool evalute problem file and fucniton
</commit_message>
<xml_diff>
--- a/languageGP/test_problems/problem_2d.xlsx
+++ b/languageGP/test_problems/problem_2d.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,10 +426,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>3258187.988484114</v>
+        <v>11405552.54744129</v>
       </c>
       <c r="C1" t="n">
-        <v>86014</v>
+        <v>708.7123800000003</v>
       </c>
     </row>
     <row r="2">
@@ -437,10 +437,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>86814</v>
+        <v>8739.481059048341</v>
       </c>
       <c r="C2" t="n">
-        <v>86014</v>
+        <v>708.7123800000003</v>
       </c>
     </row>
     <row r="3">
@@ -448,10 +448,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>86014</v>
+        <v>5680.345838510723</v>
       </c>
       <c r="C3" t="n">
-        <v>86014</v>
+        <v>708.6528799999999</v>
       </c>
     </row>
     <row r="4">
@@ -459,10 +459,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>80414</v>
+        <v>1308.687959128571</v>
       </c>
       <c r="C4" t="n">
-        <v>76014</v>
+        <v>708.6528799999999</v>
       </c>
     </row>
     <row r="5">
@@ -470,10 +470,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>76014</v>
+        <v>908.6508168000006</v>
       </c>
       <c r="C5" t="n">
-        <v>76014</v>
+        <v>708.5403</v>
       </c>
     </row>
     <row r="6">
@@ -481,10 +481,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>76014</v>
+        <v>3895.2336944</v>
       </c>
       <c r="C6" t="n">
-        <v>76014</v>
+        <v>708.5403</v>
       </c>
     </row>
     <row r="7">
@@ -492,10 +492,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>76014</v>
+        <v>2104.17944012582</v>
       </c>
       <c r="C7" t="n">
-        <v>76014</v>
+        <v>482.6313</v>
       </c>
     </row>
     <row r="8">
@@ -503,10 +503,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>76014</v>
+        <v>126973.0903128002</v>
       </c>
       <c r="C8" t="n">
-        <v>76014</v>
+        <v>481.0824</v>
       </c>
     </row>
     <row r="9">
@@ -514,10 +514,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>76414</v>
+        <v>51893.58138400123</v>
       </c>
       <c r="C9" t="n">
-        <v>76014</v>
+        <v>481.0824</v>
       </c>
     </row>
     <row r="10">
@@ -525,10 +525,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>101720.48</v>
+        <v>683.7364411594712</v>
       </c>
       <c r="C10" t="n">
-        <v>76014</v>
+        <v>480.0564000000001</v>
       </c>
     </row>
     <row r="11">
@@ -536,10 +536,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>102121.36</v>
+        <v>489.6572348000001</v>
       </c>
       <c r="C11" t="n">
-        <v>76014</v>
+        <v>479.9304000000001</v>
       </c>
     </row>
     <row r="12">
@@ -547,10 +547,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>76014</v>
+        <v>2670.4397992</v>
       </c>
       <c r="C12" t="n">
-        <v>76014</v>
+        <v>479.9304000000001</v>
       </c>
     </row>
     <row r="13">
@@ -558,10 +558,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>76014</v>
+        <v>903.7085683999995</v>
       </c>
       <c r="C13" t="n">
-        <v>76014</v>
+        <v>479.862</v>
       </c>
     </row>
     <row r="14">
@@ -569,10 +569,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>76014</v>
+        <v>278170.4863760102</v>
       </c>
       <c r="C14" t="n">
-        <v>76014</v>
+        <v>479.862</v>
       </c>
     </row>
     <row r="15">
@@ -580,10 +580,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>101720.24</v>
+        <v>493.6244012000001</v>
       </c>
       <c r="C15" t="n">
-        <v>76014</v>
+        <v>479.862</v>
       </c>
     </row>
     <row r="16">
@@ -591,10 +591,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>76014</v>
+        <v>489.0565904000001</v>
       </c>
       <c r="C16" t="n">
-        <v>76014</v>
+        <v>479.862</v>
       </c>
     </row>
     <row r="17">
@@ -602,10 +602,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>76014</v>
+        <v>502.7851600029607</v>
       </c>
       <c r="C17" t="n">
-        <v>76014</v>
+        <v>479.862</v>
       </c>
     </row>
     <row r="18">
@@ -613,10 +613,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>76014</v>
+        <v>892.16312</v>
       </c>
       <c r="C18" t="n">
-        <v>76014</v>
+        <v>479.862</v>
       </c>
     </row>
     <row r="19">
@@ -624,10 +624,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>101720.24</v>
+        <v>1113.419829639337</v>
       </c>
       <c r="C19" t="n">
-        <v>76014</v>
+        <v>473.3266743356361</v>
       </c>
     </row>
     <row r="20">
@@ -635,10 +635,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>76014</v>
+        <v>19778.57796962079</v>
       </c>
       <c r="C20" t="n">
-        <v>76014</v>
+        <v>470.998</v>
       </c>
     </row>
     <row r="21">
@@ -646,10 +646,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>76014</v>
+        <v>258286.6450773514</v>
       </c>
       <c r="C21" t="n">
-        <v>76014</v>
+        <v>470.998</v>
       </c>
     </row>
     <row r="22">
@@ -657,10 +657,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>76014</v>
+        <v>1084.204412208857</v>
       </c>
       <c r="C22" t="n">
-        <v>76014</v>
+        <v>470.998</v>
       </c>
     </row>
     <row r="23">
@@ -668,10 +668,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>76014</v>
+        <v>749.8044458096717</v>
       </c>
       <c r="C23" t="n">
-        <v>76014</v>
+        <v>470.998</v>
       </c>
     </row>
     <row r="24">
@@ -679,10 +679,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>101720.24</v>
+        <v>509135.8728313679</v>
       </c>
       <c r="C24" t="n">
-        <v>76014</v>
+        <v>470.998</v>
       </c>
     </row>
     <row r="25">
@@ -690,10 +690,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>76014</v>
+        <v>477.182343251326</v>
       </c>
       <c r="C25" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="26">
@@ -701,10 +701,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>101723.2</v>
+        <v>225649.5543293998</v>
       </c>
       <c r="C26" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="27">
@@ -712,10 +712,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>76414</v>
+        <v>1202.597914147074</v>
       </c>
       <c r="C27" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="28">
@@ -723,10 +723,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>76014</v>
+        <v>168968.9559923781</v>
       </c>
       <c r="C28" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="29">
@@ -734,10 +734,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>76014</v>
+        <v>731.2922805818179</v>
       </c>
       <c r="C29" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="30">
@@ -745,10 +745,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>76014</v>
+        <v>876.1576839065034</v>
       </c>
       <c r="C30" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="31">
@@ -756,10 +756,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>76014</v>
+        <v>4081579.514292036</v>
       </c>
       <c r="C31" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="32">
@@ -767,10 +767,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>76014</v>
+        <v>485.6508555636361</v>
       </c>
       <c r="C32" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="33">
@@ -778,10 +778,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>76014</v>
+        <v>221276.1309744256</v>
       </c>
       <c r="C33" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="34">
@@ -789,10 +789,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>76014</v>
+        <v>376900.0786442182</v>
       </c>
       <c r="C34" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="35">
@@ -800,10 +800,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>76014</v>
+        <v>470.9979999999996</v>
       </c>
       <c r="C35" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="36">
@@ -811,10 +811,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>76014</v>
+        <v>470.9979999999996</v>
       </c>
       <c r="C36" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="37">
@@ -822,10 +822,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>76014</v>
+        <v>2666.749721068997</v>
       </c>
       <c r="C37" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="38">
@@ -833,10 +833,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>76014</v>
+        <v>520091.8911429781</v>
       </c>
       <c r="C38" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="39">
@@ -844,10 +844,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>76014</v>
+        <v>356892.2616799998</v>
       </c>
       <c r="C39" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="40">
@@ -855,10 +855,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>76414</v>
+        <v>470.9979999999996</v>
       </c>
       <c r="C40" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="41">
@@ -866,10 +866,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>92668.72</v>
+        <v>1085.9559452</v>
       </c>
       <c r="C41" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="42">
@@ -877,10 +877,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>76414</v>
+        <v>127503.2351233978</v>
       </c>
       <c r="C42" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="43">
@@ -888,10 +888,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>76414</v>
+        <v>696.7315199999997</v>
       </c>
       <c r="C43" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="44">
@@ -899,10 +899,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>101720.24</v>
+        <v>2661.578039999999</v>
       </c>
       <c r="C44" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="45">
@@ -910,10 +910,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>76414</v>
+        <v>134783.2940366016</v>
       </c>
       <c r="C45" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="46">
@@ -921,10 +921,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>76014</v>
+        <v>470.9979999999996</v>
       </c>
       <c r="C46" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="47">
@@ -932,10 +932,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>76014</v>
+        <v>764.8754408</v>
       </c>
       <c r="C47" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="48">
@@ -943,10 +943,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>76014</v>
+        <v>887.0396141212118</v>
       </c>
       <c r="C48" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="49">
@@ -954,10 +954,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>76414</v>
+        <v>676.3557748671514</v>
       </c>
       <c r="C49" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="50">
@@ -965,10 +965,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>76014</v>
+        <v>190157.009167386</v>
       </c>
       <c r="C50" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="51">
@@ -976,10 +976,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>76014</v>
+        <v>475.8152442181815</v>
       </c>
       <c r="C51" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="52">
@@ -987,10 +987,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>76014</v>
+        <v>1083.969896166424</v>
       </c>
       <c r="C52" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="53">
@@ -998,10 +998,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>76414</v>
+        <v>471.582334230727</v>
       </c>
       <c r="C53" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="54">
@@ -1009,10 +1009,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>76014</v>
+        <v>471.510559563636</v>
       </c>
       <c r="C54" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="55">
@@ -1020,10 +1020,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>76014</v>
+        <v>399675.7538315486</v>
       </c>
       <c r="C55" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="56">
@@ -1031,10 +1031,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>76014</v>
+        <v>475.8114042181815</v>
       </c>
       <c r="C56" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="57">
@@ -1042,10 +1042,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>118827.76</v>
+        <v>200591.7996191394</v>
       </c>
       <c r="C57" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="58">
@@ -1053,10 +1053,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>76014</v>
+        <v>726.5448568121209</v>
       </c>
       <c r="C58" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="59">
@@ -1064,10 +1064,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>76014</v>
+        <v>471.4943563485451</v>
       </c>
       <c r="C59" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="60">
@@ -1075,10 +1075,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>76014</v>
+        <v>480.6294434671326</v>
       </c>
       <c r="C60" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="61">
@@ -1086,10 +1086,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>76414</v>
+        <v>222554.4777116358</v>
       </c>
       <c r="C61" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="62">
@@ -1097,10 +1097,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>76414</v>
+        <v>895.7628456111986</v>
       </c>
       <c r="C62" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="63">
@@ -1108,10 +1108,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>444947.6624</v>
+        <v>471.2073199999997</v>
       </c>
       <c r="C63" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="64">
@@ -1119,10 +1119,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>76014</v>
+        <v>758.7556034709492</v>
       </c>
       <c r="C64" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="65">
@@ -1130,10 +1130,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>76014</v>
+        <v>770.6859642239681</v>
       </c>
       <c r="C65" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="66">
@@ -1141,10 +1141,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>76414</v>
+        <v>475.7519199999996</v>
       </c>
       <c r="C66" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="67">
@@ -1152,10 +1152,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>76014</v>
+        <v>470.9979999999996</v>
       </c>
       <c r="C67" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="68">
@@ -1163,10 +1163,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>76014</v>
+        <v>475.8485515636361</v>
       </c>
       <c r="C68" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="69">
@@ -1174,10 +1174,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>101727.0856</v>
+        <v>202316.9275630398</v>
       </c>
       <c r="C69" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="70">
@@ -1185,10 +1185,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>76414</v>
+        <v>470.9979999999996</v>
       </c>
       <c r="C70" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="71">
@@ -1196,10 +1196,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>76014</v>
+        <v>471.1925599999997</v>
       </c>
       <c r="C71" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="72">
@@ -1207,10 +1207,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>76014</v>
+        <v>471.2370873534509</v>
       </c>
       <c r="C72" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="73">
@@ -1218,10 +1218,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>76014</v>
+        <v>125529.4393023997</v>
       </c>
       <c r="C73" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="74">
@@ -1229,10 +1229,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>874814</v>
+        <v>135661.8055823412</v>
       </c>
       <c r="C74" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="75">
@@ -1240,10 +1240,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>101720.24</v>
+        <v>301066.7394034889</v>
       </c>
       <c r="C75" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="76">
@@ -1251,10 +1251,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>76014</v>
+        <v>190590.4388987373</v>
       </c>
       <c r="C76" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="77">
@@ -1262,10 +1262,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>76014</v>
+        <v>121275.7603864412</v>
       </c>
       <c r="C77" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="78">
@@ -1273,10 +1273,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>76414</v>
+        <v>288230.4758367509</v>
       </c>
       <c r="C78" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="79">
@@ -1284,10 +1284,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>76014</v>
+        <v>388250.1379050402</v>
       </c>
       <c r="C79" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="80">
@@ -1295,10 +1295,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>76014</v>
+        <v>114593.3963034989</v>
       </c>
       <c r="C80" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="81">
@@ -1306,10 +1306,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>76414</v>
+        <v>174286.7480601509</v>
       </c>
       <c r="C81" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="82">
@@ -1317,10 +1317,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>76014</v>
+        <v>470.9979999999996</v>
       </c>
       <c r="C82" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="83">
@@ -1328,10 +1328,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>76014</v>
+        <v>535.6898318970224</v>
       </c>
       <c r="C83" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="84">
@@ -1339,10 +1339,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>76014</v>
+        <v>143824.8617501738</v>
       </c>
       <c r="C84" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="85">
@@ -1350,10 +1350,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>76014</v>
+        <v>877.7451781024238</v>
       </c>
       <c r="C85" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="86">
@@ -1361,10 +1361,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>76414</v>
+        <v>671.2074570666663</v>
       </c>
       <c r="C86" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="87">
@@ -1372,10 +1372,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>76014</v>
+        <v>72280.09504894409</v>
       </c>
       <c r="C87" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="88">
@@ -1383,10 +1383,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>101722.7018404908</v>
+        <v>2874.256519197355</v>
       </c>
       <c r="C88" t="n">
-        <v>76014</v>
+        <v>470.9979999999999</v>
       </c>
     </row>
     <row r="89">
@@ -1394,10 +1394,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>76014</v>
+        <v>471.2448914417716</v>
       </c>
       <c r="C89" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="90">
@@ -1405,10 +1405,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>76014</v>
+        <v>471.0049127290916</v>
       </c>
       <c r="C90" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="91">
@@ -1416,10 +1416,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>76014</v>
+        <v>393664.8986329426</v>
       </c>
       <c r="C91" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="92">
@@ -1427,10 +1427,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>76014</v>
+        <v>784.0279663453726</v>
       </c>
       <c r="C92" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="93">
@@ -1438,10 +1438,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>76014</v>
+        <v>212714.7084487154</v>
       </c>
       <c r="C93" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="94">
@@ -1449,10 +1449,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>76014</v>
+        <v>360147.0672588984</v>
       </c>
       <c r="C94" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="95">
@@ -1460,10 +1460,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>76014</v>
+        <v>671.4274005501741</v>
       </c>
       <c r="C95" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="96">
@@ -1471,10 +1471,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>76014</v>
+        <v>471.2232488818091</v>
       </c>
       <c r="C96" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="97">
@@ -1482,10 +1482,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>76014</v>
+        <v>475.0081293386439</v>
       </c>
       <c r="C97" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="98">
@@ -1493,10 +1493,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>76014</v>
+        <v>749233986.6710591</v>
       </c>
       <c r="C98" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="99">
@@ -1504,10 +1504,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>76014</v>
+        <v>100691.1953993772</v>
       </c>
       <c r="C99" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
       </c>
     </row>
     <row r="100">
@@ -1515,10 +1515,1110 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>101723.2</v>
+        <v>1471.41977671683</v>
       </c>
       <c r="C100" t="n">
-        <v>76014</v>
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" t="n">
+        <v>167378.5900030376</v>
+      </c>
+      <c r="C101" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" t="n">
+        <v>476.6146444846092</v>
+      </c>
+      <c r="C102" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" t="n">
+        <v>13292627.82203033</v>
+      </c>
+      <c r="C103" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103</v>
+      </c>
+      <c r="B104" t="n">
+        <v>487.6088699768711</v>
+      </c>
+      <c r="C104" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104</v>
+      </c>
+      <c r="B105" t="n">
+        <v>1271.251687569362</v>
+      </c>
+      <c r="C105" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105</v>
+      </c>
+      <c r="B106" t="n">
+        <v>186872.4415989722</v>
+      </c>
+      <c r="C106" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106</v>
+      </c>
+      <c r="B107" t="n">
+        <v>502340.6982268008</v>
+      </c>
+      <c r="C107" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107</v>
+      </c>
+      <c r="B108" t="n">
+        <v>713243.275928598</v>
+      </c>
+      <c r="C108" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108</v>
+      </c>
+      <c r="B109" t="n">
+        <v>1077.742134942903</v>
+      </c>
+      <c r="C109" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109</v>
+      </c>
+      <c r="B110" t="n">
+        <v>334193.8301344173</v>
+      </c>
+      <c r="C110" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110</v>
+      </c>
+      <c r="B111" t="n">
+        <v>2871.612775262246</v>
+      </c>
+      <c r="C111" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111</v>
+      </c>
+      <c r="B112" t="n">
+        <v>686.8373835908643</v>
+      </c>
+      <c r="C112" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112</v>
+      </c>
+      <c r="B113" t="n">
+        <v>164115.2920547941</v>
+      </c>
+      <c r="C113" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>113</v>
+      </c>
+      <c r="B114" t="n">
+        <v>2861.578039999996</v>
+      </c>
+      <c r="C114" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>114</v>
+      </c>
+      <c r="B115" t="n">
+        <v>480.585260896574</v>
+      </c>
+      <c r="C115" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>115</v>
+      </c>
+      <c r="B116" t="n">
+        <v>685.9484475461264</v>
+      </c>
+      <c r="C116" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" t="n">
+        <v>475.8783382040841</v>
+      </c>
+      <c r="C117" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>117</v>
+      </c>
+      <c r="B118" t="n">
+        <v>133497.6378013505</v>
+      </c>
+      <c r="C118" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>118</v>
+      </c>
+      <c r="B119" t="n">
+        <v>1084.60712991256</v>
+      </c>
+      <c r="C119" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>119</v>
+      </c>
+      <c r="B120" t="n">
+        <v>471.0038872282283</v>
+      </c>
+      <c r="C120" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>120</v>
+      </c>
+      <c r="B121" t="n">
+        <v>444521.2046537054</v>
+      </c>
+      <c r="C121" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" t="n">
+        <v>111510.213449431</v>
+      </c>
+      <c r="C122" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>122</v>
+      </c>
+      <c r="B123" t="n">
+        <v>575.1678788092819</v>
+      </c>
+      <c r="C123" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>123</v>
+      </c>
+      <c r="B124" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C124" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>124</v>
+      </c>
+      <c r="B125" t="n">
+        <v>672.0627634211116</v>
+      </c>
+      <c r="C125" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>125</v>
+      </c>
+      <c r="B126" t="n">
+        <v>471.2278201339093</v>
+      </c>
+      <c r="C126" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>126</v>
+      </c>
+      <c r="B127" t="n">
+        <v>2661.578039999999</v>
+      </c>
+      <c r="C127" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>127</v>
+      </c>
+      <c r="B128" t="n">
+        <v>471.4785654145246</v>
+      </c>
+      <c r="C128" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" t="n">
+        <v>55855.27034959402</v>
+      </c>
+      <c r="C129" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129</v>
+      </c>
+      <c r="B130" t="n">
+        <v>471.0137949999997</v>
+      </c>
+      <c r="C130" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>130</v>
+      </c>
+      <c r="B131" t="n">
+        <v>2866.343285203624</v>
+      </c>
+      <c r="C131" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>131</v>
+      </c>
+      <c r="B132" t="n">
+        <v>471.2603141631997</v>
+      </c>
+      <c r="C132" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>132</v>
+      </c>
+      <c r="B133" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C133" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>133</v>
+      </c>
+      <c r="B134" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C134" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>134</v>
+      </c>
+      <c r="B135" t="n">
+        <v>499.4700042414352</v>
+      </c>
+      <c r="C135" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" t="n">
+        <v>471.0449765075099</v>
+      </c>
+      <c r="C136" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" t="n">
+        <v>365847.8717191381</v>
+      </c>
+      <c r="C137" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" t="n">
+        <v>242107.3034994839</v>
+      </c>
+      <c r="C138" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" t="n">
+        <v>475.7658986895428</v>
+      </c>
+      <c r="C139" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" t="n">
+        <v>676.0669810040843</v>
+      </c>
+      <c r="C140" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" t="n">
+        <v>2965.552580424143</v>
+      </c>
+      <c r="C141" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" t="n">
+        <v>14901.60288693151</v>
+      </c>
+      <c r="C142" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="n">
+        <v>679.0111585090349</v>
+      </c>
+      <c r="C143" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>143</v>
+      </c>
+      <c r="B144" t="n">
+        <v>1086.196000060467</v>
+      </c>
+      <c r="C144" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>144</v>
+      </c>
+      <c r="B145" t="n">
+        <v>685.9757911908642</v>
+      </c>
+      <c r="C145" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>145</v>
+      </c>
+      <c r="B146" t="n">
+        <v>209693.4942799994</v>
+      </c>
+      <c r="C146" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>146</v>
+      </c>
+      <c r="B147" t="n">
+        <v>473.1480787696863</v>
+      </c>
+      <c r="C147" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>147</v>
+      </c>
+      <c r="B148" t="n">
+        <v>81484.5331798854</v>
+      </c>
+      <c r="C148" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" t="n">
+        <v>471.2000959700558</v>
+      </c>
+      <c r="C149" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" t="n">
+        <v>471.3266301734419</v>
+      </c>
+      <c r="C150" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" t="n">
+        <v>875.8396391424169</v>
+      </c>
+      <c r="C151" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" t="n">
+        <v>199675.96076</v>
+      </c>
+      <c r="C152" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" t="n">
+        <v>477.4492418991953</v>
+      </c>
+      <c r="C153" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="n">
+        <v>1961.610607146922</v>
+      </c>
+      <c r="C154" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" t="n">
+        <v>878.1170715374175</v>
+      </c>
+      <c r="C155" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" t="n">
+        <v>7202.578644613407</v>
+      </c>
+      <c r="C156" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C157" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" t="n">
+        <v>2866.420281696572</v>
+      </c>
+      <c r="C158" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>158</v>
+      </c>
+      <c r="B159" t="n">
+        <v>3063.200049615448</v>
+      </c>
+      <c r="C159" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>159</v>
+      </c>
+      <c r="B160" t="n">
+        <v>471.2008197716146</v>
+      </c>
+      <c r="C160" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>160</v>
+      </c>
+      <c r="B161" t="n">
+        <v>475.9505199999996</v>
+      </c>
+      <c r="C161" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" t="n">
+        <v>96072.95348440474</v>
+      </c>
+      <c r="C162" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" t="n">
+        <v>475.8282416965739</v>
+      </c>
+      <c r="C163" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>163</v>
+      </c>
+      <c r="B164" t="n">
+        <v>475.8317223229722</v>
+      </c>
+      <c r="C164" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>164</v>
+      </c>
+      <c r="B165" t="n">
+        <v>3118.233815666868</v>
+      </c>
+      <c r="C165" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>165</v>
+      </c>
+      <c r="B166" t="n">
+        <v>230529.4714587049</v>
+      </c>
+      <c r="C166" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>166</v>
+      </c>
+      <c r="B167" t="n">
+        <v>2861.784471461011</v>
+      </c>
+      <c r="C167" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>167</v>
+      </c>
+      <c r="B168" t="n">
+        <v>2314996572644.241</v>
+      </c>
+      <c r="C168" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>168</v>
+      </c>
+      <c r="B169" t="n">
+        <v>684.065182713917</v>
+      </c>
+      <c r="C169" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>169</v>
+      </c>
+      <c r="B170" t="n">
+        <v>471.041644576052</v>
+      </c>
+      <c r="C170" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>170</v>
+      </c>
+      <c r="B171" t="n">
+        <v>2661.578039999999</v>
+      </c>
+      <c r="C171" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>171</v>
+      </c>
+      <c r="B172" t="n">
+        <v>683.8058922377528</v>
+      </c>
+      <c r="C172" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="n">
+        <v>3211.429024419049</v>
+      </c>
+      <c r="C173" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="n">
+        <v>2866.334159999999</v>
+      </c>
+      <c r="C174" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C175" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>175</v>
+      </c>
+      <c r="B176" t="n">
+        <v>68271.06015360969</v>
+      </c>
+      <c r="C176" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>176</v>
+      </c>
+      <c r="B177" t="n">
+        <v>471.0449765075099</v>
+      </c>
+      <c r="C177" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>177</v>
+      </c>
+      <c r="B178" t="n">
+        <v>546043.2247979667</v>
+      </c>
+      <c r="C178" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>178</v>
+      </c>
+      <c r="B179" t="n">
+        <v>476.3345737486092</v>
+      </c>
+      <c r="C179" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="n">
+        <v>214130.2116137423</v>
+      </c>
+      <c r="C180" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="n">
+        <v>471.1870916018172</v>
+      </c>
+      <c r="C181" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
+        <v>181</v>
+      </c>
+      <c r="B182" t="n">
+        <v>473.6683462788349</v>
+      </c>
+      <c r="C182" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>182</v>
+      </c>
+      <c r="B183" t="n">
+        <v>471.0026168674696</v>
+      </c>
+      <c r="C183" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>183</v>
+      </c>
+      <c r="B184" t="n">
+        <v>471.0449765075099</v>
+      </c>
+      <c r="C184" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>184</v>
+      </c>
+      <c r="B185" t="n">
+        <v>670.9979999999997</v>
+      </c>
+      <c r="C185" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>185</v>
+      </c>
+      <c r="B186" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C186" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>186</v>
+      </c>
+      <c r="B187" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C187" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>187</v>
+      </c>
+      <c r="B188" t="n">
+        <v>670.9979999999997</v>
+      </c>
+      <c r="C188" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>188</v>
+      </c>
+      <c r="B189" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C189" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>189</v>
+      </c>
+      <c r="B190" t="n">
+        <v>475.3721822107966</v>
+      </c>
+      <c r="C190" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>190</v>
+      </c>
+      <c r="B191" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C191" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
+        <v>191</v>
+      </c>
+      <c r="B192" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C192" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>192</v>
+      </c>
+      <c r="B193" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C193" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>193</v>
+      </c>
+      <c r="B194" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C194" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
+        <v>194</v>
+      </c>
+      <c r="B195" t="n">
+        <v>675.8370661663945</v>
+      </c>
+      <c r="C195" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
+        <v>195</v>
+      </c>
+      <c r="B196" t="n">
+        <v>471.1908662969001</v>
+      </c>
+      <c r="C196" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>196</v>
+      </c>
+      <c r="B197" t="n">
+        <v>493163.3076200071</v>
+      </c>
+      <c r="C197" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>197</v>
+      </c>
+      <c r="B198" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C198" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>198</v>
+      </c>
+      <c r="B199" t="n">
+        <v>470.9979999999996</v>
+      </c>
+      <c r="C199" t="n">
+        <v>470.9979999999998</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>199</v>
+      </c>
+      <c r="B200" t="n">
+        <v>670.9979999999997</v>
+      </c>
+      <c r="C200" t="n">
+        <v>470.9979999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>